<commit_message>
commited to the git
</commit_message>
<xml_diff>
--- a/Scealextric/DATA/Mitchell's Consent Requests.xlsx
+++ b/Scealextric/DATA/Mitchell's Consent Requests.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/padraigmitchell/Google Drive/Fourth Year/Final Year Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/padraigmitchell/git/Scealextric/Scealextric/DATA/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="5060" windowWidth="11880" windowHeight="12860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,232 +27,229 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
-  <si>
-    <t>Conset Request</t>
-  </si>
-  <si>
-    <t>Would you like a story?</t>
-  </si>
-  <si>
-    <t>Want a story?</t>
-  </si>
-  <si>
-    <t>Fancy a story?</t>
-  </si>
-  <si>
-    <t>How about a story?</t>
-  </si>
-  <si>
-    <t>Would you like me to tell you a story?</t>
-  </si>
-  <si>
-    <t>Want me to tell you a story?</t>
-  </si>
-  <si>
-    <t>Fancy a story told by me?</t>
-  </si>
-  <si>
-    <t>How about I tell you a story?</t>
-  </si>
-  <si>
-    <t>Would you like me to tweet you a story?</t>
-  </si>
-  <si>
-    <t>Fancy a story in tweets?</t>
-  </si>
-  <si>
-    <t>Want a story in tweets?</t>
-  </si>
-  <si>
-    <t>How about I tweet you a story?</t>
-  </si>
-  <si>
-    <t>Would you like an entertaining story?</t>
-  </si>
-  <si>
-    <t>Want an entertaining story?</t>
-  </si>
-  <si>
-    <t>Fancy an entertaining story?</t>
-  </si>
-  <si>
-    <t>How about a entertaining story?</t>
-  </si>
-  <si>
-    <t>Would you like me to tell you an entertaining story?</t>
-  </si>
-  <si>
-    <t>Want me to tell you an entertaining story?</t>
-  </si>
-  <si>
-    <t>Fancy an entertaining story told by me?</t>
-  </si>
-  <si>
-    <t>How about I tell you an entertaining story?</t>
-  </si>
-  <si>
-    <t>Would you like me to tweet you an entertaing story</t>
-  </si>
-  <si>
-    <t>Want an entertaining story in tweets?</t>
-  </si>
-  <si>
-    <t>How about I tweet you an entertaining story?</t>
-  </si>
-  <si>
-    <t>Fancy an entertaining story in tweets?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot, would you like a story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot, want a story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot, fancy a story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot, how about a story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot, would you like me to tell you a story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot, want me to tell you a story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot, fancy a story told by me?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot, how about I tell you a story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot, would you like me to tweet you story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot,  want a story in tweets?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot, fancy a story in tweets?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot, how about I tweet you a story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot, would you like an entertaining story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot, want an entertaining story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot, fancy an entertaining story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot, how about an entertaining story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot, would you like me to tell you an entertaining story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot, want me to tell you an entertaining story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot, fancy an entertaining story told by me?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot, how about I tell you an entertaining story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot, would you like me to tweet you an entertaining story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot, want an entertaining story in tweets?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot, fancy an entertaining story in tweets?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hi I'm a Twitter Twitterbot, how about I tweet you an entertaining story? </t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot from @ucddublin, fancy a story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot from @ucddublin, would you like a story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot from @ucddublin, want a story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot from @ucddublin, how about a story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot from @ucddublin, would you like me to tell you a story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot from @ucddublin, want me to tell you a story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot from @ucddublin, fancy a story told by me?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot from @ucddublin, how about I tell you a story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot from @ucddublin, would you like me to tweet you story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot from @ucddublin,  want a story in tweets?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot from @ucddublin, fancy a story in tweets?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot from @ucddublin, how about I tweet you a story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot from @ucddublin, would you like an entertaining story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot from @ucddublin, want an entertaining story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot from @ucddublin, fancy an entertaining story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot from @ucddublin, how about an entertaining story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot from @ucddublin, would you like me to tell you an entertaining story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot from @ucddublin, want me to tell you an entertaining story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot from @ucddublin, fancy an entertaining story told by me?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot from @ucddublin, how about I tell you an entertaining story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot from @ucddublin, would you like me to tweet you an entertaining story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot from @ucddublin, want an entertaining story in tweets?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitter Twitterbot from @ucddublin, fancy an entertaining story in tweets?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hi I'm a Twitter Twitterbot from @ucddublin, how about I tweet you an entertaining story? </t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="72">
+  <si>
+    <t>Consent Request</t>
+  </si>
+  <si>
+    <t>Reply "Yes" if you would like a story?</t>
+  </si>
+  <si>
+    <t>Reply "Yes" if you want a story?</t>
+  </si>
+  <si>
+    <t>Reply "Yes" if you fancy a story?</t>
+  </si>
+  <si>
+    <t>Reply "Yes" if you’re up for a story?</t>
+  </si>
+  <si>
+    <t>Reply "Yes" if you would like me to tell you a story?</t>
+  </si>
+  <si>
+    <t>Reply "Yes" if you want me to tell you a story?</t>
+  </si>
+  <si>
+    <t>Reply "Yes" if you fancy a story told by me?</t>
+  </si>
+  <si>
+    <t>Reply "Yes" if you would like me to tweet you a story?</t>
+  </si>
+  <si>
+    <t>Reply "Yes" if you want a story in tweets?</t>
+  </si>
+  <si>
+    <t>Reply "Yes" if you fancy a story in tweets?</t>
+  </si>
+  <si>
+    <t>Reply "Yes" if you’re up for me tweeting you a story?</t>
+  </si>
+  <si>
+    <t>Reply "Yes" if you would like an entertaining story?</t>
+  </si>
+  <si>
+    <t>Reply "Yes" if you want an entertaining story?</t>
+  </si>
+  <si>
+    <t>Reply "Yes" if you fancy an entertaining story?</t>
+  </si>
+  <si>
+    <t>Reply "Yes" if you’re up for an entertaining story?</t>
+  </si>
+  <si>
+    <t>Reply "Yes" if you would like me to tell you an entertaining story?</t>
+  </si>
+  <si>
+    <t>Reply "Yes" if you want me to tell you an entertaining story?</t>
+  </si>
+  <si>
+    <t>Reply "Yes" if you fancy an entertaining story told by me?</t>
+  </si>
+  <si>
+    <t>Reply "Yes" if you’re up for me telling you an entertaining story?</t>
+  </si>
+  <si>
+    <t>Reply "Yes" if you would like me to tweet you an entertaining story</t>
+  </si>
+  <si>
+    <t>Reply "Yes" if you want an entertaining story in tweets?</t>
+  </si>
+  <si>
+    <t>Reply "Yes" if you fancy an entertaining story in tweets?</t>
+  </si>
+  <si>
+    <t>Reply "Yes" if you’re up for me tweeting you an entertaining story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitter Twitterbot,  reply "Yes" if you would like a story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitter Twitterbot, reply "Yes" if you want a story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitter Twitterbot, reply "Yes" if you fancy a story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitter Twitterbot, reply "Yes" if you’re up for a story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitter Twitterbot, reply "Yes" if you would like me to tell you a story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitter Twitterbot, reply "Yes" if you want me to tell you a story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitter Twitterbot, reply "Yes" if you fancy a story told by me?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitter Twitterbot, reply "Yes" if you’re up for me telling you a story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitter Twitterbot, reply "Yes" if you would like me to tweet you story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitter Twitterbot,  reply "Yes" want a story in tweets?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitter Twitterbot, reply "Yes" if you fancy a story in tweets?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitter Twitterbot, reply "Yes" if you want me to tweet you a story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitter Twitterbot, reply "Yes" if you would like an entertaining story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitter Twitterbot, reply "Yes" if you want an entertaining story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitter Twitterbot, reply "Yes" if you fancy an entertaining story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitter Twitterbot, reply "Yes" if you’re up for an entertaining story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitter Twitterbot, reply "Yes" if you would like me to tell you an entertaining story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitter Twitterbot, reply "Yes" if you want me to tell you an entertaining story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitter Twitterbot, reply "Yes" if you fancy an entertaining story told by me?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitter Twitterbot, reply "Yes"  if you’re up for me telling you an entertaining story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitter Twitterbot, reply "Yes" if you would like me to tweet you an entertaining story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitter Twitterbot, reply "Yes" if you want an entertaining story in tweets?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitter Twitterbot, reply "Yes" if you fancy an entertaining story in tweets?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot, reply "Yes" if you’re up for me tweeting you an entertaining story? </t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitter Twitterbot from @ucddublin, reply "Yes" if you would you like a story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitter Twitterbot from @ucddublin, reply "Yes" if you want a story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitter Twitterbot from @ucddublin, reply "Yes" if you fancy a story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitter Twitterbot from @ucddublin, reply "Yes" if you’re up for a story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitter Twitterbot from @ucddublin, reply "Yes" if you would like me to tell you a story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitter Twitterbot from @ucddublin, reply "Yes" if you want me to tell you a story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitter Twitterbot from @ucddublin, reply "Yes" if you fancy a story told by me?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitter Twitterbot from @ucddublin, reply "Yes" if you’re up for me telling you a story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitter Twitterbot from @ucddublin, reply "Yes" if  you would like me to tweet you story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitter Twitterbot from @ucddublin, reply "Yes" if you want a story in tweets?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitter Twitterbot from @ucddublin, reply "Yes" if you fancy a story in tweets?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitter Twitterbot from @ucddublin, reply "Yes" if you’re up for me tweeting you a story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitter Twitterbot from @ucddublin, reply "Yes" if you would like an entertaining story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitter Twitterbot from @ucddublin, reply "Yes" if you want an entertaining story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitter Twitterbot from @ucddublin, reply "Yes" if you fancy an entertaining story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitter Twitterbot from @ucddublin, reply "Yes" for an entertaining story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitter Twitterbot from @ucddublin, reply "Yes" if you would like me to tell you an entertaining story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitter Twitterbot from @ucddublin, reply "Yes" if you want me to tell you an entertaining story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitter Twitterbot from @ucddublin, reply "Yes" if you fancy an entertaining story told by me?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitter Twitterbot from @ucddublin, reply "Yes" for me to tell you an entertaining story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitter Twitterbot from @ucddublin, reply "Yes" if you would like me to tweet you an entertaining story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitter Twitterbot from @ucddublin, reply "Yes" if you want an entertaining story in tweets?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitter Twitterbot from @ucddublin, reply "Yes" if you fancy an entertaining story in tweets?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitter Twitterbot from @ucddublin, reply "Yes" for me to tweet you an entertaining story? </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -263,9 +260,14 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -289,9 +291,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -572,7 +579,7 @@
   <dimension ref="A1:A73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B10"/>
+      <selection sqref="A1:A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -587,363 +594,363 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" s="2" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Categorising user and using caterorisation to choose characters and starting actions. Classes set up and tested Needs to be intergrated
</commit_message>
<xml_diff>
--- a/Scealextric/DATA/Mitchell's Consent Requests.xlsx
+++ b/Scealextric/DATA/Mitchell's Consent Requests.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/padraigmitchell/git/Scealextric/Scealextric/DATA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/padraigmitchell/git/EntertainMe/Scealextric/DATA/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -173,76 +173,76 @@
     <t xml:space="preserve">Hi I'm a Twitterbot, reply "YES" if you’re up for me tweeting you an entertaining story? </t>
   </si>
   <si>
-    <t>Hi I'm a Twitterbot from UCD Dublin, reply "YES" if you would you like a story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitterbot from UCD Dublin, reply "YES" if you want a story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitterbot from UCD Dublin, reply "YES" if you fancy a story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitterbot from UCD Dublin, reply "YES" if you’re up for a story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitterbot from UCD Dublin, reply "YES" if you would like me to tell you a story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitterbot from UCD Dublin, reply "YES" if you want me to tell you a story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitterbot from UCD Dublin, reply "YES" if you fancy a story told by me?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitterbot from UCD Dublin, reply "YES" if you’re up for me telling you a story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitterbot from UCD Dublin, reply "YES" if  you would like me to tweet you story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitterbot from UCD Dublin, reply "YES" if you want a story in tweets?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitterbot from UCD Dublin, reply "YES" if you fancy a story in tweets?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitterbot from UCD Dublin, reply "YES" if you’re up for me tweeting you a story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitterbot from UCD Dublin, reply "YES" if you would like an entertaining story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitterbot from UCD Dublin, reply "YES" if you want an entertaining story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitterbot from UCD Dublin, reply "YES" if you fancy an entertaining story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitterbot from UCD Dublin, reply "YES" for an entertaining story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitterbot from UCD Dublin, reply "YES" if you would like me to tell you an entertaining story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitterbot from UCD Dublin, reply "YES" if you want me to tell you an entertaining story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitterbot from UCD Dublin, reply "YES" if you fancy an entertaining story told by me?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitterbot from UCD Dublin, reply "YES" for me to tell you an entertaining story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitterbot from UCD Dublin, reply "YES" if you would like me to tweet you an entertaining story?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitterbot from UCD Dublin, reply "YES" if you want an entertaining story in tweets?</t>
-  </si>
-  <si>
-    <t>Hi I'm a Twitterbot from UCD Dublin, reply "YES" if you fancy an entertaining story in tweets?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hi I'm a Twitterbot from UCD Dublin, reply "YES" for me to tweet you an entertaining story? </t>
+    <t>Hi I'm a Twitterbot from UCD Comp Sci, reply "YES" if you would you like a story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitterbot from UCD Comp Sci, reply "YES" if you want a story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitterbot from UCD Comp Sci, reply "YES" if you fancy a story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitterbot from UCD Comp Sci, reply "YES" if you’re up for a story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitterbot from UCD Comp Sci, reply "YES" if you would like me to tell you a story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitterbot from UCD Comp Sci, reply "YES" if you want me to tell you a story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitterbot from UCD Comp Sci, reply "YES" if you fancy a story told by me?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitterbot from UCD Comp Sci, reply "YES" if you’re up for me telling you a story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitterbot from UCD Comp Sci, reply "YES" if  you would like me to tweet you story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitterbot from UCD Comp Sci, reply "YES" if you want a story in tweets?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitterbot from UCD Comp Sci, reply "YES" if you fancy a story in tweets?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitterbot from UCD Comp Sci, reply "YES" if you’re up for me tweeting you a story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitterbot from UCD Comp Sci, reply "YES" if you would like an entertaining story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitterbot from UCD Comp Sci, reply "YES" if you want an entertaining story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitterbot from UCD Comp Sci, reply "YES" if you fancy an entertaining story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitterbot from UCD Comp Sci, reply "YES" for an entertaining story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitterbot from UCD Comp Sci, reply "YES" if you would like me to tell you an entertaining story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitterbot from UCD Comp Sci, reply "YES" if you want me to tell you an entertaining story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitterbot from UCD Comp Sci, reply "YES" if you fancy an entertaining story told by me?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitterbot from UCD Comp Sci, reply "YES" for me to tell you an entertaining story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitterbot from UCD Comp Sci, reply "YES" if you would like me to tweet you an entertaining story?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitterbot from UCD Comp Sci, reply "YES" if you want an entertaining story in tweets?</t>
+  </si>
+  <si>
+    <t>Hi I'm a Twitterbot from UCD Comp Sci, reply "YES" if you fancy an entertaining story in tweets?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I'm a Twitterbot from UCD Comp Sci, reply "YES" for me to tweet you an entertaining story? </t>
   </si>
 </sst>
 </file>
@@ -578,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="A65" sqref="A1:A73"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>